<commit_message>
Plot addition for assignment completion
</commit_message>
<xml_diff>
--- a/data/GOZO_assignment_count.xlsx
+++ b/data/GOZO_assignment_count.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GOZO/participant_3_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1EA60BE-3DB4-DA4E-A855-B7DDB7FFC5EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB9C511-5567-4C4F-802F-564FD1F13FF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30700" yWindow="2500" windowWidth="28800" windowHeight="16420" xr2:uid="{2FF04964-7F32-AF41-A5F9-FFB2D5CCFF2D}"/>
+    <workbookView xWindow="1640" yWindow="1120" windowWidth="28800" windowHeight="16420" xr2:uid="{2FF04964-7F32-AF41-A5F9-FFB2D5CCFF2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,24 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
-    <t>Session</t>
+    <t>session</t>
   </si>
   <si>
-    <t>Count</t>
+    <t>completed</t>
   </si>
   <si>
-    <t>10 out of 40</t>
-  </si>
-  <si>
-    <t>10 out of 38</t>
-  </si>
-  <si>
-    <t>15 out of 42</t>
-  </si>
-  <si>
-    <t>22 out of 48</t>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -402,52 +393,67 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD5B556-9057-0343-A18D-6714DE7E2CA0}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
+      <c r="B2">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
+      <c r="B3">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
+      <c r="B4">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>5</v>
+      <c r="B5">
+        <v>22</v>
+      </c>
+      <c r="C5">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Data update for status tracking goal session 5
</commit_message>
<xml_diff>
--- a/data/GOZO_assignment_count.xlsx
+++ b/data/GOZO_assignment_count.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jimwright/Desktop/University of Oregon Courses/Dissertation/Dissertation Clients/GOZO/participant_3_data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A16BE2F-3433-AA4B-903D-9A7EDD4A031B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD06A8C-101A-9947-A7C1-F325BF67CFD2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34060" yWindow="2580" windowWidth="28800" windowHeight="16300" xr2:uid="{2FF04964-7F32-AF41-A5F9-FFB2D5CCFF2D}"/>
   </bookViews>
@@ -461,10 +461,10 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>